<commit_message>
Actualización modelo_af 2022 en ceros
Se actualiza el archivo modelo_af poniendo 2022, año atipico de caida en ceros
</commit_message>
<xml_diff>
--- a/Modelo_af.xlsx
+++ b/Modelo_af.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laura\Desktop\Andres Florez\ARCAD\Arkad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Thinkpad E14\Documents\GitHub\Arkad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AE1F2C-F164-4851-9FF5-3F697965334E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{449F275E-F793-4FEE-AF75-7AD1313B39A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFA501B6-8271-423C-A00F-145B11D41630}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CFA501B6-8271-423C-A00F-145B11D41630}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B853"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D365" sqref="D365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,7 +465,7 @@
         <v>44562</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -473,7 +473,7 @@
         <v>44563</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -481,7 +481,7 @@
         <v>44564</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -489,7 +489,7 @@
         <v>44565</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -497,7 +497,7 @@
         <v>44566</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -505,7 +505,7 @@
         <v>44567</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -513,7 +513,7 @@
         <v>44568</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>44569</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>44570</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>44571</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
         <v>44572</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v>44573</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>44574</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -569,7 +569,7 @@
         <v>44575</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -577,7 +577,7 @@
         <v>44576</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
         <v>44577</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -593,7 +593,7 @@
         <v>44578</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -601,7 +601,7 @@
         <v>44579</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>44580</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>44581</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -625,7 +625,7 @@
         <v>44582</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -633,7 +633,7 @@
         <v>44583</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -641,7 +641,7 @@
         <v>44584</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
         <v>44585</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -657,7 +657,7 @@
         <v>44586</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -665,7 +665,7 @@
         <v>44587</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -673,7 +673,7 @@
         <v>44588</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
         <v>44589</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -689,7 +689,7 @@
         <v>44590</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>44591</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -705,7 +705,7 @@
         <v>44592</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -713,7 +713,7 @@
         <v>44593</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>44594</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
         <v>44595</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -737,7 +737,7 @@
         <v>44596</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
         <v>44597</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -753,7 +753,7 @@
         <v>44598</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -761,7 +761,7 @@
         <v>44599</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -769,7 +769,7 @@
         <v>44600</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -777,7 +777,7 @@
         <v>44601</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -785,7 +785,7 @@
         <v>44602</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -793,7 +793,7 @@
         <v>44603</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -801,7 +801,7 @@
         <v>44604</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -809,7 +809,7 @@
         <v>44605</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -817,7 +817,7 @@
         <v>44606</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -825,7 +825,7 @@
         <v>44607</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -833,7 +833,7 @@
         <v>44608</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -841,7 +841,7 @@
         <v>44609</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -849,7 +849,7 @@
         <v>44610</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -857,7 +857,7 @@
         <v>44611</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>44612</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -873,7 +873,7 @@
         <v>44613</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -881,7 +881,7 @@
         <v>44614</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -889,7 +889,7 @@
         <v>44615</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -897,7 +897,7 @@
         <v>44616</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -905,7 +905,7 @@
         <v>44617</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>44618</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -921,7 +921,7 @@
         <v>44619</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -929,7 +929,7 @@
         <v>44620</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -937,7 +937,7 @@
         <v>44621</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -945,7 +945,7 @@
         <v>44622</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>44623</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -961,7 +961,7 @@
         <v>44624</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -969,7 +969,7 @@
         <v>44625</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
         <v>44626</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -985,7 +985,7 @@
         <v>44627</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -993,7 +993,7 @@
         <v>44628</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1001,7 +1001,7 @@
         <v>44629</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
         <v>44630</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1017,7 +1017,7 @@
         <v>44631</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1025,7 +1025,7 @@
         <v>44632</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1033,7 +1033,7 @@
         <v>44633</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
         <v>44634</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
         <v>44635</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1057,7 +1057,7 @@
         <v>44636</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1065,7 +1065,7 @@
         <v>44637</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1073,7 +1073,7 @@
         <v>44638</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1081,7 +1081,7 @@
         <v>44639</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1089,7 +1089,7 @@
         <v>44640</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1097,7 +1097,7 @@
         <v>44641</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1105,7 +1105,7 @@
         <v>44642</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1113,7 +1113,7 @@
         <v>44643</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1121,7 +1121,7 @@
         <v>44644</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1129,7 +1129,7 @@
         <v>44645</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1137,7 +1137,7 @@
         <v>44646</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1145,7 +1145,7 @@
         <v>44647</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
         <v>44648</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1161,7 +1161,7 @@
         <v>44649</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1169,7 +1169,7 @@
         <v>44650</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
         <v>44651</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1185,7 +1185,7 @@
         <v>44652</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>44653</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1201,7 +1201,7 @@
         <v>44654</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
         <v>44655</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
         <v>44656</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
         <v>44657</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1233,7 @@
         <v>44658</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>44659</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
         <v>44660</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1257,7 +1257,7 @@
         <v>44661</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -1265,7 +1265,7 @@
         <v>44662</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
         <v>44663</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -1281,7 +1281,7 @@
         <v>44664</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>44665</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>44666</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1305,7 +1305,7 @@
         <v>44667</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -1313,7 +1313,7 @@
         <v>44668</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -1321,7 +1321,7 @@
         <v>44669</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -1329,7 +1329,7 @@
         <v>44670</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -1337,7 +1337,7 @@
         <v>44671</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -1345,7 +1345,7 @@
         <v>44672</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -1353,7 +1353,7 @@
         <v>44673</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -1361,7 +1361,7 @@
         <v>44674</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -1369,7 +1369,7 @@
         <v>44675</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -1377,7 +1377,7 @@
         <v>44676</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -1385,7 +1385,7 @@
         <v>44677</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -1393,7 +1393,7 @@
         <v>44678</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -1401,7 +1401,7 @@
         <v>44679</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -1409,7 +1409,7 @@
         <v>44680</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -1417,7 +1417,7 @@
         <v>44681</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -1425,7 +1425,7 @@
         <v>44682</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -1433,7 +1433,7 @@
         <v>44683</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
         <v>44684</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -1449,7 +1449,7 @@
         <v>44685</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
         <v>44686</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
         <v>44687</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -1473,7 +1473,7 @@
         <v>44688</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -1481,7 +1481,7 @@
         <v>44689</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -1489,7 +1489,7 @@
         <v>44690</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -1497,7 +1497,7 @@
         <v>44691</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -1505,7 +1505,7 @@
         <v>44692</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -1513,7 +1513,7 @@
         <v>44693</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -1521,7 +1521,7 @@
         <v>44694</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -1529,7 +1529,7 @@
         <v>44695</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -1537,7 +1537,7 @@
         <v>44696</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -1545,7 +1545,7 @@
         <v>44697</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -1553,7 +1553,7 @@
         <v>44698</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -1561,7 +1561,7 @@
         <v>44699</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -1569,7 +1569,7 @@
         <v>44700</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -1577,7 +1577,7 @@
         <v>44701</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -1585,7 +1585,7 @@
         <v>44702</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -1593,7 +1593,7 @@
         <v>44703</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -1601,7 +1601,7 @@
         <v>44704</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -1609,7 +1609,7 @@
         <v>44705</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -1617,7 +1617,7 @@
         <v>44706</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -1625,7 +1625,7 @@
         <v>44707</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -1633,7 +1633,7 @@
         <v>44708</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -1641,7 +1641,7 @@
         <v>44709</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -1649,7 +1649,7 @@
         <v>44710</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -1657,7 +1657,7 @@
         <v>44711</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -1665,7 +1665,7 @@
         <v>44712</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -1673,7 +1673,7 @@
         <v>44713</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -1681,7 +1681,7 @@
         <v>44714</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -1689,7 +1689,7 @@
         <v>44715</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -1697,7 +1697,7 @@
         <v>44716</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -1705,7 +1705,7 @@
         <v>44717</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -1713,7 +1713,7 @@
         <v>44718</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -1721,7 +1721,7 @@
         <v>44719</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -1729,7 +1729,7 @@
         <v>44720</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -1737,7 +1737,7 @@
         <v>44721</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -1745,7 +1745,7 @@
         <v>44722</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -1753,7 +1753,7 @@
         <v>44723</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -1761,7 +1761,7 @@
         <v>44724</v>
       </c>
       <c r="B164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -1769,7 +1769,7 @@
         <v>44725</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -1777,7 +1777,7 @@
         <v>44726</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -1785,7 +1785,7 @@
         <v>44727</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -1793,7 +1793,7 @@
         <v>44728</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -1801,7 +1801,7 @@
         <v>44729</v>
       </c>
       <c r="B169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -1809,7 +1809,7 @@
         <v>44730</v>
       </c>
       <c r="B170">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -1817,7 +1817,7 @@
         <v>44731</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -1825,7 +1825,7 @@
         <v>44732</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -1833,7 +1833,7 @@
         <v>44733</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>44734</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -1849,7 +1849,7 @@
         <v>44735</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
         <v>44736</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
@@ -1865,7 +1865,7 @@
         <v>44737</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -1873,7 +1873,7 @@
         <v>44738</v>
       </c>
       <c r="B178">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -1881,7 +1881,7 @@
         <v>44739</v>
       </c>
       <c r="B179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -1889,7 +1889,7 @@
         <v>44740</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -1897,7 +1897,7 @@
         <v>44741</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -1905,7 +1905,7 @@
         <v>44742</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -1913,7 +1913,7 @@
         <v>44743</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -1921,7 +1921,7 @@
         <v>44744</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -1929,7 +1929,7 @@
         <v>44745</v>
       </c>
       <c r="B185">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -1937,7 +1937,7 @@
         <v>44746</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
@@ -1945,7 +1945,7 @@
         <v>44747</v>
       </c>
       <c r="B187">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -1953,7 +1953,7 @@
         <v>44748</v>
       </c>
       <c r="B188">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -1961,7 +1961,7 @@
         <v>44749</v>
       </c>
       <c r="B189">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -1969,7 +1969,7 @@
         <v>44750</v>
       </c>
       <c r="B190">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -1977,7 +1977,7 @@
         <v>44751</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -1985,7 +1985,7 @@
         <v>44752</v>
       </c>
       <c r="B192">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -1993,7 +1993,7 @@
         <v>44753</v>
       </c>
       <c r="B193">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -2001,7 +2001,7 @@
         <v>44754</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -2009,7 +2009,7 @@
         <v>44755</v>
       </c>
       <c r="B195">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -2017,7 +2017,7 @@
         <v>44756</v>
       </c>
       <c r="B196">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -2025,7 +2025,7 @@
         <v>44757</v>
       </c>
       <c r="B197">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -2033,7 +2033,7 @@
         <v>44758</v>
       </c>
       <c r="B198">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2041,7 +2041,7 @@
         <v>44759</v>
       </c>
       <c r="B199">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -2049,7 +2049,7 @@
         <v>44760</v>
       </c>
       <c r="B200">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -2057,7 +2057,7 @@
         <v>44761</v>
       </c>
       <c r="B201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -2065,7 +2065,7 @@
         <v>44762</v>
       </c>
       <c r="B202">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -2073,7 +2073,7 @@
         <v>44763</v>
       </c>
       <c r="B203">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2081,7 @@
         <v>44764</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -2089,7 +2089,7 @@
         <v>44765</v>
       </c>
       <c r="B205">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -2097,7 +2097,7 @@
         <v>44766</v>
       </c>
       <c r="B206">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -2105,7 +2105,7 @@
         <v>44767</v>
       </c>
       <c r="B207">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
         <v>44768</v>
       </c>
       <c r="B208">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -2121,7 +2121,7 @@
         <v>44769</v>
       </c>
       <c r="B209">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -2129,7 +2129,7 @@
         <v>44770</v>
       </c>
       <c r="B210">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -2137,7 +2137,7 @@
         <v>44771</v>
       </c>
       <c r="B211">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
         <v>44772</v>
       </c>
       <c r="B212">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -2153,7 +2153,7 @@
         <v>44773</v>
       </c>
       <c r="B213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -2161,7 +2161,7 @@
         <v>44774</v>
       </c>
       <c r="B214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
@@ -2169,7 +2169,7 @@
         <v>44775</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -2177,7 +2177,7 @@
         <v>44776</v>
       </c>
       <c r="B216">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -2185,7 +2185,7 @@
         <v>44777</v>
       </c>
       <c r="B217">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -2193,7 +2193,7 @@
         <v>44778</v>
       </c>
       <c r="B218">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -2201,7 +2201,7 @@
         <v>44779</v>
       </c>
       <c r="B219">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -2209,7 +2209,7 @@
         <v>44780</v>
       </c>
       <c r="B220">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
@@ -2217,7 +2217,7 @@
         <v>44781</v>
       </c>
       <c r="B221">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -2225,7 +2225,7 @@
         <v>44782</v>
       </c>
       <c r="B222">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
@@ -2233,7 +2233,7 @@
         <v>44783</v>
       </c>
       <c r="B223">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -2241,7 +2241,7 @@
         <v>44784</v>
       </c>
       <c r="B224">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -2249,7 +2249,7 @@
         <v>44785</v>
       </c>
       <c r="B225">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -2257,7 +2257,7 @@
         <v>44786</v>
       </c>
       <c r="B226">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -2265,7 +2265,7 @@
         <v>44787</v>
       </c>
       <c r="B227">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -2273,7 +2273,7 @@
         <v>44788</v>
       </c>
       <c r="B228">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -2281,7 +2281,7 @@
         <v>44789</v>
       </c>
       <c r="B229">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -2289,7 +2289,7 @@
         <v>44790</v>
       </c>
       <c r="B230">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
@@ -2297,7 +2297,7 @@
         <v>44791</v>
       </c>
       <c r="B231">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -2305,7 +2305,7 @@
         <v>44792</v>
       </c>
       <c r="B232">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -2313,7 +2313,7 @@
         <v>44793</v>
       </c>
       <c r="B233">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -2321,7 +2321,7 @@
         <v>44794</v>
       </c>
       <c r="B234">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
@@ -2329,7 +2329,7 @@
         <v>44795</v>
       </c>
       <c r="B235">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
@@ -2337,7 +2337,7 @@
         <v>44796</v>
       </c>
       <c r="B236">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -2345,7 +2345,7 @@
         <v>44797</v>
       </c>
       <c r="B237">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -2353,7 +2353,7 @@
         <v>44798</v>
       </c>
       <c r="B238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -2361,7 +2361,7 @@
         <v>44799</v>
       </c>
       <c r="B239">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -2369,7 +2369,7 @@
         <v>44800</v>
       </c>
       <c r="B240">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -2377,7 +2377,7 @@
         <v>44801</v>
       </c>
       <c r="B241">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
@@ -2385,7 +2385,7 @@
         <v>44802</v>
       </c>
       <c r="B242">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
@@ -2393,7 +2393,7 @@
         <v>44803</v>
       </c>
       <c r="B243">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -2401,7 +2401,7 @@
         <v>44804</v>
       </c>
       <c r="B244">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -2409,7 +2409,7 @@
         <v>44805</v>
       </c>
       <c r="B245">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -2417,7 +2417,7 @@
         <v>44806</v>
       </c>
       <c r="B246">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -2425,7 +2425,7 @@
         <v>44807</v>
       </c>
       <c r="B247">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -2433,7 +2433,7 @@
         <v>44808</v>
       </c>
       <c r="B248">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -2441,7 +2441,7 @@
         <v>44809</v>
       </c>
       <c r="B249">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -2449,7 +2449,7 @@
         <v>44810</v>
       </c>
       <c r="B250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -2457,7 +2457,7 @@
         <v>44811</v>
       </c>
       <c r="B251">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -2465,7 +2465,7 @@
         <v>44812</v>
       </c>
       <c r="B252">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -2473,7 +2473,7 @@
         <v>44813</v>
       </c>
       <c r="B253">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -2481,7 +2481,7 @@
         <v>44814</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -2489,7 +2489,7 @@
         <v>44815</v>
       </c>
       <c r="B255">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -2497,7 +2497,7 @@
         <v>44816</v>
       </c>
       <c r="B256">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -2505,7 +2505,7 @@
         <v>44817</v>
       </c>
       <c r="B257">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -2513,7 +2513,7 @@
         <v>44818</v>
       </c>
       <c r="B258">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -2521,7 +2521,7 @@
         <v>44819</v>
       </c>
       <c r="B259">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -2529,7 +2529,7 @@
         <v>44820</v>
       </c>
       <c r="B260">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -2537,7 +2537,7 @@
         <v>44821</v>
       </c>
       <c r="B261">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -2545,7 +2545,7 @@
         <v>44822</v>
       </c>
       <c r="B262">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -2553,7 +2553,7 @@
         <v>44823</v>
       </c>
       <c r="B263">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -2561,7 +2561,7 @@
         <v>44824</v>
       </c>
       <c r="B264">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -2569,7 +2569,7 @@
         <v>44825</v>
       </c>
       <c r="B265">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -2577,7 +2577,7 @@
         <v>44826</v>
       </c>
       <c r="B266">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -2585,7 +2585,7 @@
         <v>44827</v>
       </c>
       <c r="B267">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -2593,7 +2593,7 @@
         <v>44828</v>
       </c>
       <c r="B268">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -2601,7 +2601,7 @@
         <v>44829</v>
       </c>
       <c r="B269">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -2609,7 +2609,7 @@
         <v>44830</v>
       </c>
       <c r="B270">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
@@ -2617,7 +2617,7 @@
         <v>44831</v>
       </c>
       <c r="B271">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
@@ -2625,7 +2625,7 @@
         <v>44832</v>
       </c>
       <c r="B272">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
@@ -2633,7 +2633,7 @@
         <v>44833</v>
       </c>
       <c r="B273">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -2641,7 +2641,7 @@
         <v>44834</v>
       </c>
       <c r="B274">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
@@ -2649,7 +2649,7 @@
         <v>44835</v>
       </c>
       <c r="B275">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -2657,7 +2657,7 @@
         <v>44836</v>
       </c>
       <c r="B276">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
@@ -2665,7 +2665,7 @@
         <v>44837</v>
       </c>
       <c r="B277">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
@@ -2673,7 +2673,7 @@
         <v>44838</v>
       </c>
       <c r="B278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
@@ -2681,7 +2681,7 @@
         <v>44839</v>
       </c>
       <c r="B279">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
@@ -2689,7 +2689,7 @@
         <v>44840</v>
       </c>
       <c r="B280">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
@@ -2697,7 +2697,7 @@
         <v>44841</v>
       </c>
       <c r="B281">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -2705,7 +2705,7 @@
         <v>44842</v>
       </c>
       <c r="B282">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
@@ -2713,7 +2713,7 @@
         <v>44843</v>
       </c>
       <c r="B283">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
         <v>44844</v>
       </c>
       <c r="B284">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -2729,7 +2729,7 @@
         <v>44845</v>
       </c>
       <c r="B285">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -2737,7 +2737,7 @@
         <v>44846</v>
       </c>
       <c r="B286">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
@@ -2745,7 +2745,7 @@
         <v>44847</v>
       </c>
       <c r="B287">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
@@ -2753,7 +2753,7 @@
         <v>44848</v>
       </c>
       <c r="B288">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
@@ -2761,7 +2761,7 @@
         <v>44849</v>
       </c>
       <c r="B289">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
@@ -2769,7 +2769,7 @@
         <v>44850</v>
       </c>
       <c r="B290">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
@@ -2777,7 +2777,7 @@
         <v>44851</v>
       </c>
       <c r="B291">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
@@ -2785,7 +2785,7 @@
         <v>44852</v>
       </c>
       <c r="B292">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -2793,7 +2793,7 @@
         <v>44853</v>
       </c>
       <c r="B293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
@@ -2801,7 +2801,7 @@
         <v>44854</v>
       </c>
       <c r="B294">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
@@ -2809,7 +2809,7 @@
         <v>44855</v>
       </c>
       <c r="B295">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
@@ -2817,7 +2817,7 @@
         <v>44856</v>
       </c>
       <c r="B296">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
@@ -2825,7 +2825,7 @@
         <v>44857</v>
       </c>
       <c r="B297">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
@@ -2833,7 +2833,7 @@
         <v>44858</v>
       </c>
       <c r="B298">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
@@ -2841,7 +2841,7 @@
         <v>44859</v>
       </c>
       <c r="B299">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
@@ -2849,7 +2849,7 @@
         <v>44860</v>
       </c>
       <c r="B300">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
@@ -2857,7 +2857,7 @@
         <v>44861</v>
       </c>
       <c r="B301">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
@@ -2865,7 +2865,7 @@
         <v>44862</v>
       </c>
       <c r="B302">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
@@ -2873,7 +2873,7 @@
         <v>44863</v>
       </c>
       <c r="B303">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
@@ -2881,7 +2881,7 @@
         <v>44864</v>
       </c>
       <c r="B304">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
@@ -2889,7 +2889,7 @@
         <v>44865</v>
       </c>
       <c r="B305">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
@@ -2897,7 +2897,7 @@
         <v>44866</v>
       </c>
       <c r="B306">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
@@ -2905,7 +2905,7 @@
         <v>44867</v>
       </c>
       <c r="B307">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
@@ -2913,7 +2913,7 @@
         <v>44868</v>
       </c>
       <c r="B308">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
@@ -2921,7 +2921,7 @@
         <v>44869</v>
       </c>
       <c r="B309">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
@@ -2929,7 +2929,7 @@
         <v>44870</v>
       </c>
       <c r="B310">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
@@ -2937,7 +2937,7 @@
         <v>44871</v>
       </c>
       <c r="B311">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -2945,7 +2945,7 @@
         <v>44872</v>
       </c>
       <c r="B312">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
         <v>44873</v>
       </c>
       <c r="B313">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
@@ -2961,7 +2961,7 @@
         <v>44874</v>
       </c>
       <c r="B314">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
@@ -2969,7 +2969,7 @@
         <v>44875</v>
       </c>
       <c r="B315">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -2977,7 +2977,7 @@
         <v>44876</v>
       </c>
       <c r="B316">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
@@ -2985,7 +2985,7 @@
         <v>44877</v>
       </c>
       <c r="B317">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -2993,7 +2993,7 @@
         <v>44878</v>
       </c>
       <c r="B318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
@@ -3001,7 +3001,7 @@
         <v>44879</v>
       </c>
       <c r="B319">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
@@ -3009,7 +3009,7 @@
         <v>44880</v>
       </c>
       <c r="B320">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
@@ -3017,7 +3017,7 @@
         <v>44881</v>
       </c>
       <c r="B321">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -3025,7 +3025,7 @@
         <v>44882</v>
       </c>
       <c r="B322">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -3033,7 +3033,7 @@
         <v>44883</v>
       </c>
       <c r="B323">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -3041,7 +3041,7 @@
         <v>44884</v>
       </c>
       <c r="B324">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -3049,7 +3049,7 @@
         <v>44885</v>
       </c>
       <c r="B325">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -3057,7 +3057,7 @@
         <v>44886</v>
       </c>
       <c r="B326">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -3065,7 +3065,7 @@
         <v>44887</v>
       </c>
       <c r="B327">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
@@ -3073,7 +3073,7 @@
         <v>44888</v>
       </c>
       <c r="B328">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -3081,7 +3081,7 @@
         <v>44889</v>
       </c>
       <c r="B329">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
@@ -3089,7 +3089,7 @@
         <v>44890</v>
       </c>
       <c r="B330">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -3097,7 +3097,7 @@
         <v>44891</v>
       </c>
       <c r="B331">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -3105,7 +3105,7 @@
         <v>44892</v>
       </c>
       <c r="B332">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -3113,7 +3113,7 @@
         <v>44893</v>
       </c>
       <c r="B333">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -3121,7 +3121,7 @@
         <v>44894</v>
       </c>
       <c r="B334">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -3129,7 +3129,7 @@
         <v>44895</v>
       </c>
       <c r="B335">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -3137,7 +3137,7 @@
         <v>44896</v>
       </c>
       <c r="B336">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -3145,7 +3145,7 @@
         <v>44897</v>
       </c>
       <c r="B337">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
         <v>44898</v>
       </c>
       <c r="B338">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -3161,7 +3161,7 @@
         <v>44899</v>
       </c>
       <c r="B339">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
@@ -3169,7 +3169,7 @@
         <v>44900</v>
       </c>
       <c r="B340">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -3177,7 +3177,7 @@
         <v>44901</v>
       </c>
       <c r="B341">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
@@ -3185,7 +3185,7 @@
         <v>44902</v>
       </c>
       <c r="B342">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -3193,7 +3193,7 @@
         <v>44903</v>
       </c>
       <c r="B343">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -3201,7 +3201,7 @@
         <v>44904</v>
       </c>
       <c r="B344">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
@@ -3209,7 +3209,7 @@
         <v>44905</v>
       </c>
       <c r="B345">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
@@ -3217,7 +3217,7 @@
         <v>44906</v>
       </c>
       <c r="B346">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
@@ -3225,7 +3225,7 @@
         <v>44907</v>
       </c>
       <c r="B347">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
@@ -3233,7 +3233,7 @@
         <v>44908</v>
       </c>
       <c r="B348">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
@@ -3241,7 +3241,7 @@
         <v>44909</v>
       </c>
       <c r="B349">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -3249,7 +3249,7 @@
         <v>44910</v>
       </c>
       <c r="B350">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
@@ -3257,7 +3257,7 @@
         <v>44911</v>
       </c>
       <c r="B351">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
@@ -3265,7 +3265,7 @@
         <v>44912</v>
       </c>
       <c r="B352">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
@@ -3273,7 +3273,7 @@
         <v>44913</v>
       </c>
       <c r="B353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
@@ -3281,7 +3281,7 @@
         <v>44914</v>
       </c>
       <c r="B354">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
@@ -3289,7 +3289,7 @@
         <v>44915</v>
       </c>
       <c r="B355">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
@@ -3297,7 +3297,7 @@
         <v>44916</v>
       </c>
       <c r="B356">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
@@ -3305,7 +3305,7 @@
         <v>44917</v>
       </c>
       <c r="B357">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
@@ -3313,7 +3313,7 @@
         <v>44918</v>
       </c>
       <c r="B358">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
@@ -3321,7 +3321,7 @@
         <v>44919</v>
       </c>
       <c r="B359">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
@@ -3329,7 +3329,7 @@
         <v>44920</v>
       </c>
       <c r="B360">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
@@ -3337,7 +3337,7 @@
         <v>44921</v>
       </c>
       <c r="B361">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
@@ -3345,7 +3345,7 @@
         <v>44922</v>
       </c>
       <c r="B362">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
@@ -3353,7 +3353,7 @@
         <v>44923</v>
       </c>
       <c r="B363">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
@@ -3361,7 +3361,7 @@
         <v>44924</v>
       </c>
       <c r="B364">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
@@ -3369,7 +3369,7 @@
         <v>44925</v>
       </c>
       <c r="B365">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
@@ -3377,7 +3377,7 @@
         <v>44926</v>
       </c>
       <c r="B366">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>